<commit_message>
Re ran many graphs
And this is up to date with DH experiment data.  Also changed the output
file to show hours the slope of loss of Al covers.
</commit_message>
<xml_diff>
--- a/ACLData/Current expt log.xlsx
+++ b/ACLData/Current expt log.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17490" windowHeight="9405"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15210" windowHeight="8580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
   <si>
     <t>Without</t>
   </si>
@@ -32,7 +32,28 @@
     <t>With</t>
   </si>
   <si>
-    <t>Re-do, this one was shorted</t>
+    <t>overlap, cm^2</t>
+  </si>
+  <si>
+    <t>Cathode width (mm)</t>
+  </si>
+  <si>
+    <t>Anode width (mm)</t>
+  </si>
+  <si>
+    <t>Defect?</t>
+  </si>
+  <si>
+    <t>Current (nA)</t>
+  </si>
+  <si>
+    <t>Current Density (nA/cm^2)</t>
+  </si>
+  <si>
+    <t>with cosmetic tape</t>
+  </si>
+  <si>
+    <t>Backside defect</t>
   </si>
 </sst>
 </file>
@@ -68,10 +89,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -352,23 +382,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:M26"/>
+  <dimension ref="B3:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9:K17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="13" max="13" width="9.140625" style="2"/>
+    <col min="11" max="11" width="9.140625" style="2"/>
+    <col min="12" max="12" width="14.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H3" s="1">
         <v>53.083632915738001</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>4.1358999999999999E-7</v>
       </c>
@@ -381,7 +412,7 @@
         <v>8760</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>2.2607799999999999E-8</v>
       </c>
@@ -394,7 +425,7 @@
         <v>5.1369863013698627E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>6.5166599E-3</v>
       </c>
@@ -403,15 +434,33 @@
         <v>6516659.9000000004</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="1">
+    <row r="8" spans="2:14" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
         <v>5.4076287000000003E-8</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="3">
         <v>53.083632915738001</v>
       </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>3.69E-8</v>
       </c>
@@ -419,6 +468,14 @@
         <f t="shared" si="0"/>
         <v>36.9</v>
       </c>
+      <c r="E9">
+        <f>0.3*H9/10</f>
+        <v>0.15</v>
+      </c>
+      <c r="F9">
+        <f>H9/10*I9/10</f>
+        <v>0.95</v>
+      </c>
       <c r="G9">
         <v>111</v>
       </c>
@@ -434,8 +491,12 @@
       <c r="K9" s="2">
         <v>0.35269999171337502</v>
       </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L9" s="2">
+        <f>IF(J9="Without",K9/F9,K9/E9)</f>
+        <v>0.37126314917197373</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>7.3399999999999999E-9</v>
       </c>
@@ -443,6 +504,14 @@
         <f t="shared" si="0"/>
         <v>7.34</v>
       </c>
+      <c r="E10">
+        <f t="shared" ref="E10:E28" si="1">0.3*H10/10</f>
+        <v>0.57000000000000006</v>
+      </c>
+      <c r="F10">
+        <f t="shared" ref="F10:F28" si="2">H10/10*I10/10</f>
+        <v>28.689999999999998</v>
+      </c>
       <c r="G10">
         <v>231</v>
       </c>
@@ -458,8 +527,12 @@
       <c r="K10" s="2">
         <v>5.7716374473684198</v>
       </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L10" s="2">
+        <f t="shared" ref="L10:L28" si="3">IF(J10="Without",K10/F10,K10/E10)</f>
+        <v>0.20117244501109866</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>4.5499999999999997E-8</v>
       </c>
@@ -467,6 +540,14 @@
         <f t="shared" si="0"/>
         <v>45.5</v>
       </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>0.57000000000000006</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>9.69</v>
+      </c>
       <c r="G11">
         <v>222</v>
       </c>
@@ -482,8 +563,12 @@
       <c r="K11" s="2">
         <v>351.39405266666603</v>
       </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L11" s="2">
+        <f t="shared" si="3"/>
+        <v>616.48079415204563</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>2.1500000000000001E-7</v>
       </c>
@@ -491,6 +576,14 @@
         <f t="shared" si="0"/>
         <v>215</v>
       </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>1.5299999999999998</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="2"/>
+        <v>26.009999999999998</v>
+      </c>
       <c r="G12">
         <v>322</v>
       </c>
@@ -506,8 +599,20 @@
       <c r="K12" s="2">
         <v>577.60528955172401</v>
       </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L12" s="2">
+        <f t="shared" si="3"/>
+        <v>377.51979709263014</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>0.57000000000000006</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>3.6100000000000003</v>
+      </c>
       <c r="G13">
         <v>212</v>
       </c>
@@ -523,8 +628,20 @@
       <c r="K13" s="2">
         <v>350.40756454166598</v>
       </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L13" s="2">
+        <f t="shared" si="3"/>
+        <v>614.75011323099284</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>1.5299999999999998</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="2"/>
+        <v>77.009999999999991</v>
+      </c>
       <c r="G14">
         <v>331</v>
       </c>
@@ -538,13 +655,23 @@
         <v>0</v>
       </c>
       <c r="K14" s="2">
-        <v>2440.2972709000001</v>
-      </c>
-      <c r="L14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="L14" s="2">
+        <f t="shared" si="3"/>
+        <v>1.1232307492533438E-2</v>
+      </c>
+      <c r="N14" s="1"/>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>0.15</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>2.5499999999999998</v>
+      </c>
       <c r="G15">
         <v>122</v>
       </c>
@@ -560,8 +687,13 @@
       <c r="K15" s="2">
         <v>87.975533999999897</v>
       </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L15" s="2">
+        <f t="shared" si="3"/>
+        <v>586.50355999999931</v>
+      </c>
+      <c r="N15" s="1"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>24</v>
       </c>
@@ -571,6 +703,14 @@
       <c r="D16" s="1">
         <v>-4.0457099705499003E-2</v>
       </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>0.15</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
       <c r="G16">
         <v>112</v>
       </c>
@@ -584,10 +724,14 @@
         <v>1</v>
       </c>
       <c r="K16" s="2">
-        <v>133.574523888888</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+        <v>117.07350451851801</v>
+      </c>
+      <c r="L16" s="2">
+        <f>IF(J16="Without",K16/F16,K16/E16)</f>
+        <v>780.49003012345338</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>25</v>
       </c>
@@ -597,6 +741,14 @@
       <c r="D17" s="1">
         <v>-9.7901509034713594E-3</v>
       </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>1.5299999999999998</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="2"/>
+        <v>9.69</v>
+      </c>
       <c r="G17">
         <v>311</v>
       </c>
@@ -610,10 +762,14 @@
         <v>0</v>
       </c>
       <c r="K17" s="2">
-        <v>1.46783339999999</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+        <v>1.50695921588888</v>
+      </c>
+      <c r="L17" s="2">
+        <f>IF(J17="Without",K17/F17,K17/E17)</f>
+        <v>0.15551694694415688</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>26</v>
       </c>
@@ -623,6 +779,14 @@
       <c r="D18" s="1">
         <v>-8.7731918479546894E-2</v>
       </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>1.5299999999999998</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="2"/>
+        <v>9.69</v>
+      </c>
       <c r="G18">
         <v>312</v>
       </c>
@@ -635,8 +799,15 @@
       <c r="J18" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K18" s="2">
+        <v>774.11189340999999</v>
+      </c>
+      <c r="L18" s="2">
+        <f t="shared" si="3"/>
+        <v>505.95548588888897</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>27</v>
       </c>
@@ -646,6 +817,14 @@
       <c r="D19" s="1">
         <v>-1.55861612780117E-2</v>
       </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>0.15</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="2"/>
+        <v>2.5499999999999998</v>
+      </c>
       <c r="G19">
         <v>121</v>
       </c>
@@ -658,8 +837,15 @@
       <c r="J19" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K19" s="2">
+        <v>1.5221039774</v>
+      </c>
+      <c r="L19" s="2">
+        <f t="shared" si="3"/>
+        <v>0.59690352054901963</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>28</v>
       </c>
@@ -669,6 +855,14 @@
       <c r="D20" s="1">
         <v>-1.88139279480866E-2</v>
       </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>1.5299999999999998</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="2"/>
+        <v>26.009999999999998</v>
+      </c>
       <c r="G20">
         <v>321</v>
       </c>
@@ -681,8 +875,15 @@
       <c r="J20" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K20" s="2">
+        <v>0.98599439899999997</v>
+      </c>
+      <c r="L20" s="2">
+        <f t="shared" si="3"/>
+        <v>3.7908281391772394E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>29</v>
       </c>
@@ -692,6 +893,14 @@
       <c r="D21" s="1">
         <v>-9.4263398031310494E-2</v>
       </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>0.57000000000000006</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="2"/>
+        <v>28.689999999999998</v>
+      </c>
       <c r="G21">
         <v>232</v>
       </c>
@@ -704,8 +913,23 @@
       <c r="J21" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K21" s="2">
+        <v>319.54588781249902</v>
+      </c>
+      <c r="L21" s="2">
+        <f t="shared" si="3"/>
+        <v>560.6068207236824</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>0.15</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="2"/>
+        <v>7.55</v>
+      </c>
       <c r="G22">
         <v>132</v>
       </c>
@@ -718,8 +942,23 @@
       <c r="J22" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K22" s="2">
+        <v>83.655579227272696</v>
+      </c>
+      <c r="L22" s="2">
+        <f t="shared" si="3"/>
+        <v>557.70386151515129</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>0.57000000000000006</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="2"/>
+        <v>3.6100000000000003</v>
+      </c>
       <c r="G23">
         <v>211</v>
       </c>
@@ -732,8 +971,23 @@
       <c r="J23" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K23" s="2">
+        <v>9.7703686634999904</v>
+      </c>
+      <c r="L23" s="2">
+        <f t="shared" si="3"/>
+        <v>2.706473313988917</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>0.57000000000000006</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="2"/>
+        <v>9.69</v>
+      </c>
       <c r="G24">
         <v>221</v>
       </c>
@@ -746,8 +1000,23 @@
       <c r="J24" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K24" s="2">
+        <v>7.6</v>
+      </c>
+      <c r="L24" s="2">
+        <f t="shared" si="3"/>
+        <v>0.78431372549019607</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>1.5299999999999998</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="2"/>
+        <v>77.009999999999991</v>
+      </c>
       <c r="G25">
         <v>332</v>
       </c>
@@ -760,8 +1029,23 @@
       <c r="J25" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K25" s="2">
+        <v>844</v>
+      </c>
+      <c r="L25" s="2">
+        <f t="shared" si="3"/>
+        <v>551.6339869281046</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>0.15</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="2"/>
+        <v>7.55</v>
+      </c>
       <c r="G26">
         <v>131</v>
       </c>
@@ -773,6 +1057,77 @@
       </c>
       <c r="J26" t="s">
         <v>0</v>
+      </c>
+      <c r="K26" s="2">
+        <v>5.96</v>
+      </c>
+      <c r="L26" s="2">
+        <f t="shared" si="3"/>
+        <v>0.78940397350993374</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>0.15</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+      <c r="G27">
+        <v>112</v>
+      </c>
+      <c r="H27">
+        <v>5</v>
+      </c>
+      <c r="I27">
+        <v>19</v>
+      </c>
+      <c r="J27" t="s">
+        <v>1</v>
+      </c>
+      <c r="K27" s="2">
+        <v>0.97442583418333295</v>
+      </c>
+      <c r="L27" s="2">
+        <f t="shared" si="3"/>
+        <v>6.4961722278888869</v>
+      </c>
+      <c r="M27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>0.15</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+      <c r="G28">
+        <v>113</v>
+      </c>
+      <c r="H28">
+        <v>5</v>
+      </c>
+      <c r="I28">
+        <v>19</v>
+      </c>
+      <c r="J28" t="s">
+        <v>1</v>
+      </c>
+      <c r="K28" s="2">
+        <v>6</v>
+      </c>
+      <c r="L28" s="2">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="M28" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>